<commit_message>
create .rmd to reproduce jeager2018, added transcript tpm from that study as well
</commit_message>
<xml_diff>
--- a/EngramSeqDatasetsQualitySummary.xlsx
+++ b/EngramSeqDatasetsQualitySummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angus\Desktop\PavLabEngrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DAC225-4735-44B3-A72A-ADAFAE0BD247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99053B06-3CE3-4029-991A-D2B8545BF4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F6D4CCE3-AFBC-4A29-AB90-3FB0C8BE2C62}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="157">
   <si>
     <t>Study</t>
   </si>
@@ -505,6 +505,9 @@
   </si>
   <si>
     <t>Patch-seq, no electrical recordings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not useable due to developmetnal effects and DNMT overexpression. </t>
   </si>
 </sst>
 </file>
@@ -578,52 +581,16 @@
   </cellStyles>
   <dxfs count="32">
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -648,16 +615,52 @@
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -719,15 +722,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{076EC05F-B3B2-47EE-B9C9-6814FC6DAF7F}" name="Table3" displayName="Table3" ref="A35:F54" totalsRowShown="0" headerRowDxfId="24" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{076EC05F-B3B2-47EE-B9C9-6814FC6DAF7F}" name="Table3" displayName="Table3" ref="A35:F54" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A35:F54" xr:uid="{076EC05F-B3B2-47EE-B9C9-6814FC6DAF7F}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{637D7F47-E823-458E-A840-9A35D792ECC2}" name="Types of Engram Cells Available and how to pool them" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{7621BC4E-6757-4CBD-9C57-BD0976AA7B07}" name="xLabelled-celltypes-fromhere-collectedat-afterthistask" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{55670669-7E76-4EED-B684-FF7A6A979429}" name="Column1" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{6483AEFB-819C-4452-AA89-59B3F9F858DC}" name="Column2" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{75EAE5B9-7AE8-4B52-BFBC-0FF44DE031F3}" name="Column3" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{DC99C7FD-1D38-45A1-9DB4-AC8125CC96FB}" name="Column4" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{637D7F47-E823-458E-A840-9A35D792ECC2}" name="Types of Engram Cells Available and how to pool them" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{7621BC4E-6757-4CBD-9C57-BD0976AA7B07}" name="xLabelled-celltypes-fromhere-collectedat-afterthistask" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{55670669-7E76-4EED-B684-FF7A6A979429}" name="Column1" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{6483AEFB-819C-4452-AA89-59B3F9F858DC}" name="Column2" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{75EAE5B9-7AE8-4B52-BFBC-0FF44DE031F3}" name="Column3" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{DC99C7FD-1D38-45A1-9DB4-AC8125CC96FB}" name="Column4" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -737,35 +740,35 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{632548DB-0B70-4FB0-AA05-277DEEFB9811}" name="Table4" displayName="Table4" ref="A1:P12" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:P12" xr:uid="{632548DB-0B70-4FB0-AA05-277DEEFB9811}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{45FCAC4B-EC4F-41C6-9E01-90EDBE33939F}" name="Study" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{45DDAEB7-B699-45C5-BDBB-A545BF03E0CB}" name="Useability" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{6F48BC81-B7DD-40AB-BF1B-F8B961A61481}" name="Code" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{DEFE8952-863E-478D-8DDE-F93879D09574}" name="Collection method" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{83742E29-D8A8-4159-9E49-2E849F8B1CFF}" name="Data" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{01555BBA-942E-40C6-8014-8AAED7BF30D9}" name="Metadata Quality" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{90705077-9EA3-4078-A66C-FD12D978352F}" name="Sequencing Type" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{87BDA2C8-5645-40FD-B731-91C7776087AD}" name="Cell Counts" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{FA106545-BD70-48CF-B5EF-E7D7A039219D}" name="Neuron Marker (if used)" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{E04A9ED6-A84C-46C7-B5FA-23E68F2FA99F}" name="Engram Cells" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{213A76E8-3A73-40CE-88BE-70CA214F06DB}" name="IEG Marker" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{8DCCAC0F-C79F-4625-A2A2-92372E12807E}" name="Region " dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{6B9AEBE6-42DD-41FC-A23A-B51E3590F9A7}" name="Condition" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{BCE44A22-784C-49DF-A93A-98CCEB056BF8}" name="Time Course" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{A7A96AD7-5BCB-49F5-9892-D0F017493C96}" name="Reactivated" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{8D7FEF4E-FB65-4C96-A3BB-AACCC8240BA9}" name="# Mice" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{45FCAC4B-EC4F-41C6-9E01-90EDBE33939F}" name="Study" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{45DDAEB7-B699-45C5-BDBB-A545BF03E0CB}" name="Useability" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{6F48BC81-B7DD-40AB-BF1B-F8B961A61481}" name="Code" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{DEFE8952-863E-478D-8DDE-F93879D09574}" name="Collection method" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{83742E29-D8A8-4159-9E49-2E849F8B1CFF}" name="Data" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{01555BBA-942E-40C6-8014-8AAED7BF30D9}" name="Metadata Quality" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{90705077-9EA3-4078-A66C-FD12D978352F}" name="Sequencing Type" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{87BDA2C8-5645-40FD-B731-91C7776087AD}" name="Cell Counts" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{FA106545-BD70-48CF-B5EF-E7D7A039219D}" name="Neuron Marker (if used)" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{E04A9ED6-A84C-46C7-B5FA-23E68F2FA99F}" name="Engram Cells" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{213A76E8-3A73-40CE-88BE-70CA214F06DB}" name="IEG Marker" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{8DCCAC0F-C79F-4625-A2A2-92372E12807E}" name="Region " dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{6B9AEBE6-42DD-41FC-A23A-B51E3590F9A7}" name="Condition" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{BCE44A22-784C-49DF-A93A-98CCEB056BF8}" name="Time Course" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{A7A96AD7-5BCB-49F5-9892-D0F017493C96}" name="Reactivated" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{8D7FEF4E-FB65-4C96-A3BB-AACCC8240BA9}" name="# Mice" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDFED28B-E7F3-4857-92EE-42BB6D21F8FD}" name="Table2" displayName="Table2" ref="A16:D27" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DDFED28B-E7F3-4857-92EE-42BB6D21F8FD}" name="Table2" displayName="Table2" ref="A16:D27" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A16:D27" xr:uid="{DDFED28B-E7F3-4857-92EE-42BB6D21F8FD}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EA2A5FC2-D095-4E24-9CCE-82C1D1C9837E}" name="Study" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{3C743C73-DEE2-44E6-AE8D-0B878D17B4FF}" name="Useability" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{07B40804-2389-48AF-AD3E-C0AF38E0BE31}" name="Code" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{027A6E33-F868-45F0-8348-B0BD484C48E9}" name="Issues" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{EA2A5FC2-D095-4E24-9CCE-82C1D1C9837E}" name="Study" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{3C743C73-DEE2-44E6-AE8D-0B878D17B4FF}" name="Useability" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{07B40804-2389-48AF-AD3E-C0AF38E0BE31}" name="Code" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{027A6E33-F868-45F0-8348-B0BD484C48E9}" name="Issues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1070,8 +1073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B04096B-D9D1-4B6A-AF49-EBC8355C4F32}">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1771,7 +1774,7 @@
         <v>17</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>85</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>